<commit_message>
Fix tilt=n in markdown and excel files it is ok already in csv
</commit_message>
<xml_diff>
--- a/resources/4_mei_encoding/Iberian_aquitanian_notation/AQUITANIANnotation-NClevel-HalfTorculus.xlsx
+++ b/resources/4_mei_encoding/Iberian_aquitanian_notation/AQUITANIANnotation-NClevel-HalfTorculus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mthomae/Downloads/OMR_Portuguese_Sources/resources/4_mei_encoding/Iberian_aquitanian_notation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C6DA0A0E-39BA-424A-95B3-75C66603F630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D28A5FCD-5948-824B-9999-4A427D204E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18180" yWindow="500" windowWidth="32860" windowHeight="26500" xr2:uid="{0394C6CE-5AF9-CF4B-B63B-6BC72F9E9ED6}"/>
   </bookViews>
@@ -372,13 +372,6 @@
   <si>
     <t>&lt;neume&gt;
     &lt;nc curve="c" type="cephalicus"&gt;
-        &lt;liquescent/&gt;
-    &lt;/nc&gt;
-&lt;/neume&gt;</t>
-  </si>
-  <si>
-    <t>&lt;neume&gt;
-    &lt;nc curve="c" tilt="ne"&gt;
         &lt;liquescent/&gt;
     &lt;/nc&gt;
 &lt;/neume&gt;</t>
@@ -491,6 +484,33 @@
   </si>
   <si>
     <t>TorculusEnd3</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;neume&gt;
+    &lt;nc curve="c" tilt=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t>"ne"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;
+        &lt;liquescent/&gt;
+    &lt;/nc&gt;
+&lt;/neume&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1526,8 +1546,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A001BD3-14A6-E347-AC0D-A7B160A0B128}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1606,10 +1626,10 @@
         <v>13</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>31</v>
@@ -1641,10 +1661,10 @@
         <v>16</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>31</v>
@@ -1676,10 +1696,10 @@
         <v>17</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>31</v>
@@ -1708,13 +1728,13 @@
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>31</v>
@@ -1746,10 +1766,10 @@
         <v>63</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>31</v>
@@ -1778,13 +1798,13 @@
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>31</v>
@@ -1816,10 +1836,10 @@
         <v>24</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>31</v>
@@ -1851,10 +1871,10 @@
         <v>27</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>31</v>
@@ -1868,7 +1888,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>54</v>
@@ -1877,19 +1897,19 @@
         <v>55</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="H10" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>31</v>
@@ -1903,7 +1923,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>57</v>
@@ -1912,19 +1932,19 @@
         <v>58</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G11" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="I11" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>31</v>
@@ -1932,34 +1952,34 @@
     </row>
     <row r="12" spans="1:11" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" s="3" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="I12" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>31</v>
@@ -1988,13 +2008,13 @@
         <v>1</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>31</v>
@@ -2002,34 +2022,34 @@
     </row>
     <row r="14" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14" s="6" t="e" vm="13">
         <v>#VALUE!</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="F14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="I14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>31</v>

</xml_diff>